<commit_message>
fix rincian n nominatif
</commit_message>
<xml_diff>
--- a/template/nominatif_temp.xlsx
+++ b/template/nominatif_temp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\phpexcel\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WebDev\PKL-BKD\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -359,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -418,6 +418,36 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,38 +481,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,7 +770,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,162 +794,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="45" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="44"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="53"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="45" t="s">
+      <c r="G6" s="49"/>
+      <c r="H6" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="43"/>
-      <c r="J6" s="46"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="34"/>
       <c r="K6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="45" t="s">
+      <c r="L6" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="43"/>
-      <c r="N6" s="45" t="s">
+      <c r="M6" s="33"/>
+      <c r="N6" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="43"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="35" t="s">
+      <c r="O6" s="33"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="45" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="47" t="s">
+      <c r="G7" s="50"/>
+      <c r="H7" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="49"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
       <c r="K7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="47" t="s">
+      <c r="L7" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="46"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1022,11 +1025,11 @@
         <f>SUM(K8:K10)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="43">
         <f>SUM(M8:M10)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="34"/>
+      <c r="M11" s="44"/>
       <c r="N11" s="9"/>
       <c r="O11" s="7"/>
       <c r="P11" s="31">
@@ -1110,13 +1113,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="N6:P7"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A3:Q3"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="Q6:Q7"/>
@@ -1127,6 +1123,13 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="H5:Q5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="N6:P7"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>